<commit_message>
implementar de buscar producto por nombre y devuelve una lista
</commit_message>
<xml_diff>
--- a/src/main/java/control/ventas/backend/excel/productos.xlsx
+++ b/src/main/java/control/ventas/backend/excel/productos.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
-    <t xml:space="preserve">Luiz S.A.C </t>
-  </si>
-  <si>
     <t>LISTA DE PRODUCTOS</t>
   </si>
   <si>
@@ -53,22 +50,18 @@
   </si>
   <si>
     <t>Diadora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calzados Luiz S.A.C </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -161,28 +154,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -492,180 +482,180 @@
   <dimension ref="B2:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:K10"/>
+      <selection activeCell="B2" sqref="B2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="4">
+        <v>260</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="4">
+        <v>15</v>
+      </c>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="4">
+        <v>250</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="4">
+        <v>12</v>
+      </c>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="2">
-        <v>260</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="2">
-        <v>15</v>
-      </c>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="2">
-        <v>250</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="2">
-        <v>12</v>
-      </c>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="4">
+        <v>150</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="4">
+        <v>11</v>
+      </c>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="2">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7">
         <v>150</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="2">
-        <v>11</v>
-      </c>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5">
-        <v>150</v>
-      </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5">
+      <c r="K11" s="7"/>
+      <c r="L11" s="7">
         <v>5</v>
       </c>
-      <c r="M11" s="5"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
@@ -893,12 +883,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B2:M3"/>
-    <mergeCell ref="B4:M5"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="J8:K8"/>
@@ -907,14 +899,12 @@
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="B2:M3"/>
+    <mergeCell ref="B4:M5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
agregando el atributo codigo a producto
</commit_message>
<xml_diff>
--- a/src/main/java/control/ventas/backend/excel/productos.xlsx
+++ b/src/main/java/control/ventas/backend/excel/productos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>LISTA DE PRODUCTOS</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t xml:space="preserve">Calzados Luiz S.A.C </t>
+  </si>
+  <si>
+    <t>CÓDIGO</t>
+  </si>
+  <si>
+    <t>SSD41</t>
+  </si>
+  <si>
+    <t>SSD42</t>
+  </si>
+  <si>
+    <t>SER74</t>
+  </si>
+  <si>
+    <t>SXX48</t>
   </si>
 </sst>
 </file>
@@ -154,22 +169,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -482,180 +509,190 @@
   <dimension ref="B2:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M3"/>
+      <selection activeCell="L10" sqref="L10:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="4" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="4">
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10">
         <v>260</v>
       </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="4">
+      <c r="K8" s="9"/>
+      <c r="L8" s="10">
         <v>15</v>
       </c>
-      <c r="M8" s="6"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="4" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="4">
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10">
         <v>250</v>
       </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="4">
+      <c r="K9" s="9"/>
+      <c r="L9" s="10">
         <v>12</v>
       </c>
-      <c r="M9" s="6"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="4" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="4">
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10">
         <v>150</v>
       </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="4">
+      <c r="K10" s="9"/>
+      <c r="L10" s="10">
         <v>11</v>
       </c>
-      <c r="M10" s="6"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7" t="s">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7">
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11">
         <v>150</v>
       </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7">
-        <v>5</v>
-      </c>
-      <c r="M11" s="7"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11">
+        <v>10</v>
+      </c>
+      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
@@ -886,25 +923,25 @@
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="G10:I10"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="G8:I8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="B9:F9"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G8:I8"/>
     <mergeCell ref="B2:M3"/>
     <mergeCell ref="B4:M5"/>
-    <mergeCell ref="B7:F7"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="L7:M7"/>
+    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
agregando el atributo descripcion a producto y modificando el pdf para el inventario
</commit_message>
<xml_diff>
--- a/src/main/java/control/ventas/backend/excel/productos.xlsx
+++ b/src/main/java/control/ventas/backend/excel/productos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>LISTA DE PRODUCTOS</t>
   </si>
@@ -31,43 +31,61 @@
     <t>NOMBRE PRODUCTO</t>
   </si>
   <si>
-    <t>Satire</t>
-  </si>
-  <si>
-    <t>Rabona</t>
-  </si>
-  <si>
-    <t>Nike SB</t>
-  </si>
-  <si>
-    <t>Astro Kick</t>
-  </si>
-  <si>
-    <t>Puma</t>
-  </si>
-  <si>
-    <t>Belio Bl</t>
-  </si>
-  <si>
-    <t>Diadora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calzados Luiz S.A.C </t>
-  </si>
-  <si>
     <t>CÓDIGO</t>
   </si>
   <si>
-    <t>SSD41</t>
-  </si>
-  <si>
-    <t>SSD42</t>
-  </si>
-  <si>
-    <t>SER74</t>
-  </si>
-  <si>
-    <t>SXX48</t>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store Luiz S.A.C </t>
+  </si>
+  <si>
+    <t>SER41</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>Pantalla curva full HD de 24''</t>
+  </si>
+  <si>
+    <t>AZC65</t>
+  </si>
+  <si>
+    <t>Teclado</t>
+  </si>
+  <si>
+    <t>Genius</t>
+  </si>
+  <si>
+    <t>Teclado mecánico RGB</t>
+  </si>
+  <si>
+    <t>AXC85</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Razer</t>
+  </si>
+  <si>
+    <t>Mouse gamer inalámbrico</t>
+  </si>
+  <si>
+    <t>MNL15</t>
+  </si>
+  <si>
+    <t>Impresora</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Impresora con tanque de tinta recargable</t>
   </si>
 </sst>
 </file>
@@ -105,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -165,14 +183,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -188,18 +230,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -506,209 +536,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M27"/>
+  <dimension ref="B2:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10:M10"/>
+      <selection activeCell="L11" sqref="L11:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+    </row>
+    <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+    </row>
+    <row r="5" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="5">
+        <v>315</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="5">
+        <v>1</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="H9" s="7"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="5">
+        <v>50</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="10">
-        <v>260</v>
-      </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="10">
+      <c r="M9" s="6"/>
+      <c r="N9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="10">
-        <v>250</v>
-      </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="10">
-        <v>12</v>
-      </c>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10">
-        <v>150</v>
-      </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="10">
-        <v>11</v>
-      </c>
-      <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5">
+        <v>75</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="5">
+        <v>2</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11">
-        <v>150</v>
-      </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11">
-        <v>10</v>
-      </c>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8">
+        <v>500</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8">
+        <v>1</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -722,7 +816,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -736,7 +830,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -750,7 +844,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -919,29 +1013,38 @@
       <c r="M27" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="31">
+    <mergeCell ref="N8:S8"/>
+    <mergeCell ref="N9:S9"/>
+    <mergeCell ref="N10:S10"/>
+    <mergeCell ref="N11:S11"/>
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="B2:S3"/>
+    <mergeCell ref="B4:S5"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B2:M3"/>
-    <mergeCell ref="B4:M5"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>